<commit_message>
edit docx, xlsx, templates, dll
</commit_message>
<xml_diff>
--- a/templates/13.a-Lam BA Pembukaan 2 SAMPUL.xlsx
+++ b/templates/13.a-Lam BA Pembukaan 2 SAMPUL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="8670" windowHeight="4020"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="8670" windowHeight="4020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lam Buka 1 Sampul (1)" sheetId="3" r:id="rId1"/>
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="84">
   <si>
     <t>NO.</t>
   </si>
@@ -278,37 +278,10 @@
     <t>ISI BERKAS SAMPUL I</t>
   </si>
   <si>
-    <t>COPY AKTE PENDIRIAN PERUSAHAAN DAN PERUBAHANNYA JIKA ADA</t>
-  </si>
-  <si>
-    <t>SURAT IJIN JASA KONSTRUKSI DAN SBU SIPIL, MEKANIKAL DAN ELEKTRIKAL</t>
-  </si>
-  <si>
-    <t>SURAT KETERANGAN DOMISILI PERUSAHAAN YANG MASIH BERLAKU</t>
-  </si>
-  <si>
-    <t>COPY NPWP, PKP, SKT</t>
-  </si>
-  <si>
-    <t>PAJAK TAHUN TERKAHIR (SPT/PPh) PASAL 25 ATAU PASAL 21 / PASAL 23  3BLN TERAKHIR</t>
-  </si>
-  <si>
-    <t>ISIAN KUALIFIKASI PERUSAHAAN PAKAI METERAI RP. 6000</t>
-  </si>
-  <si>
-    <t>FAKTA INTEGRITAS PAKAI METERAI RP. 6000</t>
-  </si>
-  <si>
-    <t>KESEDIAAN MENGIKUTI LELANG DENGAN CARA E-BIDING PAKAI METERAI RP. 6000</t>
-  </si>
-  <si>
     <t>TENAGA AHLI YANG DITUGASKAN</t>
   </si>
   <si>
     <t>PT PLN (PERSERO) KANTOR PUSAT</t>
-  </si>
-  <si>
-    <t>PENGESAHAN KEMENHUM DAN HAM</t>
   </si>
   <si>
     <t>METODE KESELAMATAN KERJA</t>
@@ -2471,198 +2444,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="73" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="78" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="79" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="81" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="82" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="83" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="81" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="82" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="83" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="94" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="95" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="96" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="94" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="95" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="96" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2672,21 +2453,213 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="94" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="95" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="96" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="94" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="95" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="96" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="85" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="86" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="87" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="81" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="82" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="83" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="81" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="82" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="83" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="73" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="78" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="79" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3182,7 +3155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H33" sqref="H33:L40"/>
     </sheetView>
   </sheetViews>
@@ -3195,110 +3168,110 @@
   <sheetData>
     <row r="2" spans="1:12" ht="13.5" x14ac:dyDescent="0.25">
       <c r="J2" s="102" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.5" x14ac:dyDescent="0.25">
       <c r="J3" s="102" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="103"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="125" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
+      <c r="A5" s="170" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="170"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="170"/>
+      <c r="H5" s="170"/>
+      <c r="I5" s="170"/>
+      <c r="J5" s="170"/>
+      <c r="K5" s="170"/>
     </row>
     <row r="6" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="126" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
+      <c r="A6" s="171" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="171"/>
+      <c r="C6" s="171"/>
+      <c r="D6" s="171"/>
+      <c r="E6" s="171"/>
+      <c r="F6" s="171"/>
+      <c r="G6" s="171"/>
+      <c r="H6" s="171"/>
+      <c r="I6" s="171"/>
+      <c r="J6" s="171"/>
+      <c r="K6" s="171"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="127" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="127" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="128"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="127" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="129"/>
+      <c r="B7" s="172" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="173"/>
+      <c r="D7" s="173"/>
+      <c r="E7" s="174"/>
+      <c r="F7" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="173"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="172" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="174"/>
       <c r="K7" s="105" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="L7" s="106"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="107"/>
-      <c r="B8" s="130" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="133" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="134"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="133" t="s">
+      <c r="B8" s="164" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="135"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="167" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="168"/>
+      <c r="H8" s="169"/>
+      <c r="I8" s="167" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="169"/>
       <c r="K8" s="108"/>
       <c r="L8" s="106"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="107" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="136" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="140"/>
-      <c r="H9" s="141"/>
-      <c r="I9" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="141"/>
+        <v>41</v>
+      </c>
+      <c r="B9" s="140" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="141"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="144"/>
+      <c r="H9" s="145"/>
+      <c r="I9" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="145"/>
       <c r="K9" s="108"/>
       <c r="L9" s="106"/>
     </row>
@@ -3306,121 +3279,121 @@
       <c r="A10" s="109">
         <v>1</v>
       </c>
-      <c r="B10" s="136" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="137"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="140"/>
-      <c r="H10" s="141"/>
-      <c r="I10" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="141"/>
+      <c r="B10" s="140" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="141"/>
+      <c r="D10" s="141"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="144"/>
+      <c r="H10" s="145"/>
+      <c r="I10" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="145"/>
       <c r="K10" s="108"/>
       <c r="L10" s="106"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="109"/>
-      <c r="B11" s="142" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="144"/>
-      <c r="F11" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="140"/>
-      <c r="H11" s="141"/>
-      <c r="I11" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="141"/>
+      <c r="B11" s="146" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="147"/>
+      <c r="D11" s="147"/>
+      <c r="E11" s="148"/>
+      <c r="F11" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="144"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="145"/>
       <c r="K11" s="108"/>
       <c r="L11" s="106"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="109"/>
-      <c r="B12" s="142" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="143"/>
-      <c r="D12" s="143"/>
-      <c r="E12" s="144"/>
-      <c r="F12" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="140"/>
-      <c r="H12" s="141"/>
-      <c r="I12" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="141"/>
+      <c r="B12" s="146" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="144"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="145"/>
       <c r="K12" s="108"/>
       <c r="L12" s="106"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="109"/>
-      <c r="B13" s="142" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="143"/>
-      <c r="D13" s="143"/>
-      <c r="E13" s="144"/>
-      <c r="F13" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="140"/>
-      <c r="H13" s="141"/>
-      <c r="I13" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="141"/>
+      <c r="B13" s="146" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="147"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="144"/>
+      <c r="H13" s="145"/>
+      <c r="I13" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="145"/>
       <c r="K13" s="108"/>
       <c r="L13" s="106"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="109"/>
-      <c r="B14" s="142" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="143"/>
-      <c r="D14" s="143"/>
-      <c r="E14" s="144"/>
-      <c r="F14" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="140"/>
-      <c r="H14" s="141"/>
-      <c r="I14" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" s="141"/>
+      <c r="B14" s="146" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="147"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="148"/>
+      <c r="F14" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="144"/>
+      <c r="H14" s="145"/>
+      <c r="I14" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="145"/>
       <c r="K14" s="108"/>
       <c r="L14" s="106"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="109"/>
-      <c r="B15" s="142" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="143"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="144"/>
-      <c r="F15" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="140"/>
-      <c r="H15" s="141"/>
-      <c r="I15" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="141"/>
+      <c r="B15" s="146" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="147"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="148"/>
+      <c r="F15" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="144"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="145"/>
       <c r="K15" s="108"/>
       <c r="L15" s="106"/>
     </row>
@@ -3428,21 +3401,21 @@
       <c r="A16" s="109">
         <v>2</v>
       </c>
-      <c r="B16" s="136" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="137"/>
-      <c r="D16" s="137"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="140"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="141"/>
+      <c r="B16" s="140" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="141"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="144"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="145"/>
       <c r="K16" s="108"/>
       <c r="L16" s="106"/>
     </row>
@@ -3450,21 +3423,21 @@
       <c r="A17" s="110">
         <v>3</v>
       </c>
-      <c r="B17" s="145" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="147"/>
-      <c r="F17" s="148" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="149"/>
-      <c r="H17" s="150"/>
-      <c r="I17" s="148" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="150"/>
+      <c r="B17" s="158" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="159"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="161" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="162"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="161" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="163"/>
       <c r="K17" s="111"/>
       <c r="L17" s="106"/>
     </row>
@@ -3472,21 +3445,21 @@
       <c r="A18" s="109">
         <v>4</v>
       </c>
-      <c r="B18" s="136" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="139" t="s">
+      <c r="B18" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="140"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J18" s="141"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="144"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="145"/>
       <c r="K18" s="108"/>
       <c r="L18" s="106"/>
     </row>
@@ -3494,21 +3467,21 @@
       <c r="A19" s="109">
         <v>5</v>
       </c>
-      <c r="B19" s="136" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="137"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="140"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J19" s="141"/>
+      <c r="B19" s="140" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="141"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="144"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="145"/>
       <c r="K19" s="108"/>
       <c r="L19" s="106"/>
     </row>
@@ -3516,43 +3489,43 @@
       <c r="A20" s="109">
         <v>6</v>
       </c>
-      <c r="B20" s="136" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="137"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="140"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" s="141"/>
+      <c r="B20" s="140" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="142"/>
+      <c r="F20" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="144"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="145"/>
       <c r="K20" s="108"/>
       <c r="L20" s="106"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="107" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="136" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="140"/>
-      <c r="H21" s="141"/>
-      <c r="I21" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J21" s="141"/>
+        <v>55</v>
+      </c>
+      <c r="B21" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
+      <c r="E21" s="142"/>
+      <c r="F21" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="144"/>
+      <c r="H21" s="145"/>
+      <c r="I21" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="145"/>
       <c r="K21" s="108"/>
       <c r="L21" s="106"/>
     </row>
@@ -3560,21 +3533,21 @@
       <c r="A22" s="109">
         <v>1</v>
       </c>
-      <c r="B22" s="136" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="137"/>
-      <c r="D22" s="137"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="140"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J22" s="141"/>
+      <c r="B22" s="140" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="141"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="142"/>
+      <c r="F22" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="144"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="145"/>
       <c r="K22" s="108"/>
       <c r="L22" s="106"/>
     </row>
@@ -3582,21 +3555,21 @@
       <c r="A23" s="109">
         <v>2</v>
       </c>
-      <c r="B23" s="136" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="137"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="140"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J23" s="141"/>
+      <c r="B23" s="140" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="144"/>
+      <c r="H23" s="145"/>
+      <c r="I23" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="145"/>
       <c r="K23" s="108"/>
       <c r="L23" s="106"/>
     </row>
@@ -3604,21 +3577,21 @@
       <c r="A24" s="109">
         <v>3</v>
       </c>
-      <c r="B24" s="136" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="137"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="140"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J24" s="141"/>
+      <c r="B24" s="140" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="141"/>
+      <c r="D24" s="141"/>
+      <c r="E24" s="142"/>
+      <c r="F24" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="144"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="145"/>
       <c r="K24" s="108"/>
       <c r="L24" s="106"/>
     </row>
@@ -3626,21 +3599,21 @@
       <c r="A25" s="109">
         <v>4</v>
       </c>
-      <c r="B25" s="136" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="137"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" s="140"/>
-      <c r="H25" s="141"/>
-      <c r="I25" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J25" s="141"/>
+      <c r="B25" s="140" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="141"/>
+      <c r="D25" s="141"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="144"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="145"/>
       <c r="K25" s="108"/>
       <c r="L25" s="106"/>
     </row>
@@ -3648,49 +3621,49 @@
       <c r="A26" s="109">
         <v>5</v>
       </c>
-      <c r="B26" s="136" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="137"/>
-      <c r="D26" s="137"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="140"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="J26" s="141"/>
+      <c r="B26" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="144"/>
+      <c r="H26" s="145"/>
+      <c r="I26" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="145"/>
       <c r="K26" s="108"/>
       <c r="L26" s="106"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="107"/>
-      <c r="B27" s="136"/>
-      <c r="C27" s="137"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="140"/>
-      <c r="H27" s="141"/>
-      <c r="I27" s="139"/>
-      <c r="J27" s="141"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="143"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="143"/>
+      <c r="J27" s="145"/>
       <c r="K27" s="108"/>
       <c r="L27" s="106"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="107"/>
-      <c r="B28" s="142"/>
-      <c r="C28" s="143"/>
-      <c r="D28" s="143"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="140"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="139"/>
-      <c r="J28" s="141"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="147"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="148"/>
+      <c r="F28" s="143"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="143"/>
+      <c r="J28" s="145"/>
       <c r="K28" s="108"/>
       <c r="L28" s="106"/>
     </row>
@@ -3710,157 +3683,157 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="120"/>
-      <c r="B30" s="152" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="153"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="155" t="s">
-        <v>72</v>
-      </c>
-      <c r="G30" s="156"/>
-      <c r="H30" s="157"/>
-      <c r="I30" s="155" t="s">
-        <v>41</v>
-      </c>
-      <c r="J30" s="157"/>
+      <c r="B30" s="149" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="150"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="152" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="153"/>
+      <c r="H30" s="154"/>
+      <c r="I30" s="152" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="154"/>
       <c r="K30" s="121"/>
       <c r="L30" s="106"/>
     </row>
     <row r="31" spans="1:12" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="158" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="158"/>
-      <c r="D31" s="159"/>
-      <c r="E31" s="161"/>
-      <c r="F31" s="161"/>
-      <c r="G31" s="151" t="s">
-        <v>90</v>
-      </c>
-      <c r="H31" s="151"/>
-      <c r="I31" s="151"/>
-      <c r="J31" s="151"/>
-      <c r="K31" s="151"/>
-      <c r="L31" s="151"/>
+      <c r="A31" s="155" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="155"/>
+      <c r="D31" s="156"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="139" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="139"/>
+      <c r="I31" s="139"/>
+      <c r="J31" s="139"/>
+      <c r="K31" s="139"/>
+      <c r="L31" s="139"/>
     </row>
     <row r="32" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="162" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="162"/>
-      <c r="D32" s="160"/>
-      <c r="E32" s="151"/>
-      <c r="F32" s="151"/>
-      <c r="G32" s="151" t="s">
-        <v>74</v>
-      </c>
-      <c r="H32" s="151"/>
-      <c r="I32" s="151"/>
-      <c r="J32" s="151"/>
-      <c r="K32" s="151"/>
-      <c r="L32" s="151"/>
+      <c r="A32" s="135" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="135"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="139"/>
+      <c r="G32" s="139" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="139"/>
+      <c r="I32" s="139"/>
+      <c r="J32" s="139"/>
+      <c r="K32" s="139"/>
+      <c r="L32" s="139"/>
     </row>
     <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="162" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="162"/>
+      <c r="A33" s="135" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="135"/>
       <c r="D33" s="123"/>
       <c r="F33" s="123"/>
       <c r="G33" s="123"/>
-      <c r="H33" s="197" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="197"/>
-      <c r="J33" s="198" t="s">
-        <v>77</v>
-      </c>
-      <c r="K33" s="198"/>
-      <c r="L33" s="198"/>
+      <c r="H33" s="132" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="132"/>
+      <c r="J33" s="136" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="136"/>
+      <c r="L33" s="136"/>
     </row>
     <row r="34" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="162" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="162"/>
+      <c r="A34" s="135" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="135"/>
       <c r="D34" s="123"/>
       <c r="F34" s="123"/>
       <c r="G34" s="123"/>
-      <c r="H34" s="197"/>
-      <c r="I34" s="197"/>
-      <c r="J34" s="198"/>
-      <c r="K34" s="198"/>
-      <c r="L34" s="198"/>
+      <c r="H34" s="132"/>
+      <c r="I34" s="132"/>
+      <c r="J34" s="136"/>
+      <c r="K34" s="136"/>
+      <c r="L34" s="136"/>
     </row>
     <row r="35" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="163"/>
-      <c r="B35" s="163"/>
-      <c r="D35" s="164" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="164"/>
+      <c r="A35" s="137"/>
+      <c r="B35" s="137"/>
+      <c r="D35" s="138" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="138"/>
       <c r="F35" s="123"/>
       <c r="G35" s="123"/>
-      <c r="H35" s="197"/>
-      <c r="I35" s="197"/>
-      <c r="J35" s="198"/>
-      <c r="K35" s="198"/>
-      <c r="L35" s="198"/>
+      <c r="H35" s="132"/>
+      <c r="I35" s="132"/>
+      <c r="J35" s="136"/>
+      <c r="K35" s="136"/>
+      <c r="L35" s="136"/>
     </row>
     <row r="36" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="163"/>
-      <c r="B36" s="163"/>
+      <c r="A36" s="137"/>
+      <c r="B36" s="137"/>
       <c r="D36" s="123"/>
       <c r="F36" s="123"/>
       <c r="G36" s="123"/>
-      <c r="H36" s="197"/>
-      <c r="I36" s="197"/>
-      <c r="J36" s="198"/>
-      <c r="K36" s="198"/>
-      <c r="L36" s="198"/>
+      <c r="H36" s="132"/>
+      <c r="I36" s="132"/>
+      <c r="J36" s="136"/>
+      <c r="K36" s="136"/>
+      <c r="L36" s="136"/>
     </row>
     <row r="37" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="163"/>
-      <c r="B37" s="163"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="137"/>
       <c r="D37" s="122"/>
       <c r="F37" s="123"/>
       <c r="G37" s="123"/>
-      <c r="H37" s="197"/>
-      <c r="I37" s="197"/>
-      <c r="J37" s="198"/>
-      <c r="K37" s="198"/>
-      <c r="L37" s="198"/>
+      <c r="H37" s="132"/>
+      <c r="I37" s="132"/>
+      <c r="J37" s="136"/>
+      <c r="K37" s="136"/>
+      <c r="L37" s="136"/>
     </row>
     <row r="38" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="163"/>
-      <c r="B38" s="163"/>
+      <c r="A38" s="137"/>
+      <c r="B38" s="137"/>
       <c r="D38" s="124"/>
       <c r="F38" s="123"/>
       <c r="G38" s="123"/>
-      <c r="H38" s="197"/>
-      <c r="I38" s="197"/>
-      <c r="J38" s="198"/>
-      <c r="K38" s="198"/>
-      <c r="L38" s="198"/>
+      <c r="H38" s="132"/>
+      <c r="I38" s="132"/>
+      <c r="J38" s="136"/>
+      <c r="K38" s="136"/>
+      <c r="L38" s="136"/>
     </row>
     <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="124"/>
       <c r="D39" s="122" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F39" s="123"/>
       <c r="G39" s="123"/>
-      <c r="H39" s="197" t="s">
-        <v>81</v>
-      </c>
-      <c r="I39" s="199"/>
-      <c r="J39" s="198" t="s">
-        <v>77</v>
-      </c>
-      <c r="K39" s="198"/>
-      <c r="L39" s="198"/>
+      <c r="H39" s="132" t="s">
+        <v>72</v>
+      </c>
+      <c r="I39" s="133"/>
+      <c r="J39" s="136" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="136"/>
+      <c r="L39" s="136"/>
     </row>
     <row r="40" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="124"/>
@@ -3870,15 +3843,15 @@
       <c r="D40" s="124"/>
       <c r="F40" s="123"/>
       <c r="G40" s="123"/>
-      <c r="H40" s="197" t="s">
-        <v>82</v>
-      </c>
-      <c r="I40" s="199"/>
-      <c r="J40" s="198" t="s">
-        <v>83</v>
-      </c>
-      <c r="K40" s="198"/>
-      <c r="L40" s="198"/>
+      <c r="H40" s="132" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="133"/>
+      <c r="J40" s="136" t="s">
+        <v>74</v>
+      </c>
+      <c r="K40" s="136"/>
+      <c r="L40" s="136"/>
     </row>
     <row r="41" spans="1:12" ht="13.5" x14ac:dyDescent="0.2">
       <c r="D41" s="122"/>
@@ -3887,10 +3860,10 @@
       <c r="D42" s="124"/>
     </row>
     <row r="43" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D43" s="160" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="160"/>
+      <c r="D43" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="134"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C44" s="101">
@@ -3898,30 +3871,75 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="D47" s="160" t="s">
-        <v>85</v>
-      </c>
-      <c r="E47" s="160"/>
+      <c r="D47" s="134" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="134"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="J33:L38"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="G31:L31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="I26:J26"/>
@@ -3938,65 +3956,20 @@
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:F32"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="G31:L31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="J33:L38"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4007,8 +3980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D57" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="M68" sqref="M68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4036,43 +4009,43 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="180"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
+      <c r="A2" s="175" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
+      <c r="I2" s="175"/>
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="181" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
+      <c r="A3" s="176" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="176"/>
+      <c r="G3" s="176"/>
+      <c r="H3" s="176"/>
+      <c r="I3" s="176"/>
     </row>
     <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="181" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="181"/>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
+      <c r="A4" s="176" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="176"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
+      <c r="H4" s="176"/>
+      <c r="I4" s="176"/>
     </row>
     <row r="5" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -4085,37 +4058,37 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="21" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="185" t="s">
+      <c r="A6" s="180" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="35"/>
-      <c r="C6" s="187" t="s">
+      <c r="C6" s="182" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="182" t="s">
+      <c r="D6" s="177" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="183"/>
-      <c r="F6" s="183"/>
-      <c r="G6" s="183"/>
-      <c r="H6" s="183"/>
-      <c r="I6" s="184"/>
+      <c r="E6" s="178"/>
+      <c r="F6" s="178"/>
+      <c r="G6" s="178"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="179"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="186"/>
+      <c r="A7" s="181"/>
       <c r="B7" s="36"/>
-      <c r="C7" s="188"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="81" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E7" s="82" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F7" s="82" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G7" s="82" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H7" s="82"/>
       <c r="I7" s="83"/>
@@ -4153,7 +4126,7 @@
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="61" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
@@ -4174,16 +4147,16 @@
       <c r="I10" s="71"/>
     </row>
     <row r="11" spans="1:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="175" t="s">
+      <c r="A11" s="188" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="176"/>
-      <c r="C11" s="177"/>
+      <c r="B11" s="189"/>
+      <c r="C11" s="190"/>
       <c r="D11" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>2</v>
@@ -4213,13 +4186,11 @@
       <c r="A13" s="43">
         <v>1</v>
       </c>
-      <c r="B13" s="165" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="166"/>
+      <c r="B13" s="191"/>
+      <c r="C13" s="192"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -4230,9 +4201,7 @@
       <c r="A14" s="43">
         <v>2</v>
       </c>
-      <c r="B14" s="57" t="s">
-        <v>20</v>
-      </c>
+      <c r="B14" s="57"/>
       <c r="C14" s="49"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -4245,10 +4214,8 @@
       <c r="A15" s="43">
         <v>3</v>
       </c>
-      <c r="B15" s="165" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="166"/>
+      <c r="B15" s="191"/>
+      <c r="C15" s="192"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -4260,10 +4227,8 @@
       <c r="A16" s="43">
         <v>4</v>
       </c>
-      <c r="B16" s="165" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="166"/>
+      <c r="B16" s="191"/>
+      <c r="C16" s="192"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -4275,10 +4240,8 @@
       <c r="A17" s="48">
         <v>5</v>
       </c>
-      <c r="B17" s="178" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="179"/>
+      <c r="B17" s="193"/>
+      <c r="C17" s="194"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -4290,10 +4253,8 @@
       <c r="A18" s="43">
         <v>6</v>
       </c>
-      <c r="B18" s="171" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="172"/>
+      <c r="B18" s="184"/>
+      <c r="C18" s="185"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -4305,10 +4266,8 @@
       <c r="A19" s="43">
         <v>7</v>
       </c>
-      <c r="B19" s="173" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="174"/>
+      <c r="B19" s="186"/>
+      <c r="C19" s="187"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
@@ -4320,10 +4279,8 @@
       <c r="A20" s="43">
         <v>8</v>
       </c>
-      <c r="B20" s="165" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="166"/>
+      <c r="B20" s="191"/>
+      <c r="C20" s="192"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
@@ -4335,10 +4292,8 @@
       <c r="A21" s="43">
         <v>9</v>
       </c>
-      <c r="B21" s="165" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="166"/>
+      <c r="B21" s="191"/>
+      <c r="C21" s="192"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -4350,9 +4305,7 @@
       <c r="A22" s="43">
         <v>10</v>
       </c>
-      <c r="B22" s="57" t="s">
-        <v>42</v>
-      </c>
+      <c r="B22" s="57"/>
       <c r="C22" s="49"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -4494,17 +4447,17 @@
       <c r="A32" s="22"/>
       <c r="B32" s="95"/>
       <c r="C32" s="80" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D32" s="96"/>
       <c r="E32" s="96" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F32" s="96" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G32" s="96" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H32" s="96"/>
       <c r="I32" s="97"/>
@@ -4532,7 +4485,7 @@
       </c>
       <c r="B34" s="45"/>
       <c r="C34" s="60" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="41"/>
@@ -4562,11 +4515,11 @@
       </c>
       <c r="B36" s="47"/>
       <c r="C36" s="16" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="13" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
@@ -4579,7 +4532,7 @@
       </c>
       <c r="B37" s="47"/>
       <c r="C37" s="16" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
@@ -4594,7 +4547,7 @@
       </c>
       <c r="B38" s="47"/>
       <c r="C38" s="16" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
@@ -4609,11 +4562,11 @@
       </c>
       <c r="B39" s="44"/>
       <c r="C39" s="16" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
@@ -4626,7 +4579,7 @@
       </c>
       <c r="B40" s="44"/>
       <c r="C40" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -4641,7 +4594,7 @@
       </c>
       <c r="B41" s="44"/>
       <c r="C41" s="16" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
@@ -4656,7 +4609,7 @@
       </c>
       <c r="B42" s="44"/>
       <c r="C42" s="16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
@@ -4671,7 +4624,7 @@
       </c>
       <c r="B43" s="44"/>
       <c r="C43" s="16" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
@@ -4725,14 +4678,14 @@
       <c r="A47" s="66"/>
       <c r="B47" s="67"/>
       <c r="C47" s="80" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D47" s="68"/>
       <c r="E47" s="68" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F47" s="68" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G47" s="68"/>
       <c r="H47" s="68"/>
@@ -4753,7 +4706,7 @@
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="85" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D49" s="86"/>
       <c r="E49" s="15"/>
@@ -4765,10 +4718,10 @@
     <row r="50" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
-      <c r="C50" s="169" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="170"/>
+      <c r="C50" s="198" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="199"/>
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
       <c r="G50" s="15"/>
@@ -4778,10 +4731,10 @@
     <row r="51" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
-      <c r="C51" s="169" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="170"/>
+      <c r="C51" s="198" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="199"/>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
@@ -4792,7 +4745,7 @@
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="87" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="15"/>
@@ -4839,13 +4792,13 @@
       <c r="B56" s="5"/>
       <c r="C56" s="84"/>
       <c r="D56" s="15"/>
-      <c r="E56" s="167" t="s">
-        <v>89</v>
-      </c>
-      <c r="F56" s="167"/>
-      <c r="G56" s="167"/>
-      <c r="H56" s="167"/>
-      <c r="I56" s="167"/>
+      <c r="E56" s="196" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" s="196"/>
+      <c r="G56" s="196"/>
+      <c r="H56" s="196"/>
+      <c r="I56" s="196"/>
     </row>
     <row r="57" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
@@ -4863,26 +4816,26 @@
       <c r="B58" s="5"/>
       <c r="C58" s="9"/>
       <c r="D58" s="6"/>
-      <c r="E58" s="168" t="s">
-        <v>92</v>
-      </c>
-      <c r="F58" s="168"/>
-      <c r="G58" s="168"/>
-      <c r="H58" s="168"/>
-      <c r="I58" s="168"/>
+      <c r="E58" s="197" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="197"/>
+      <c r="G58" s="197"/>
+      <c r="H58" s="197"/>
+      <c r="I58" s="197"/>
     </row>
     <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="9"/>
       <c r="D59" s="6"/>
-      <c r="E59" s="168" t="s">
+      <c r="E59" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="F59" s="168"/>
-      <c r="G59" s="168"/>
-      <c r="H59" s="168"/>
-      <c r="I59" s="168"/>
+      <c r="F59" s="197"/>
+      <c r="G59" s="197"/>
+      <c r="H59" s="197"/>
+      <c r="I59" s="197"/>
     </row>
     <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
@@ -4928,34 +4881,34 @@
       <c r="D63" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E63" s="189">
+      <c r="E63" s="125">
         <v>1</v>
       </c>
-      <c r="F63" s="190"/>
-      <c r="G63" s="190" t="s">
-        <v>2</v>
-      </c>
-      <c r="H63" s="190" t="s">
+      <c r="F63" s="126"/>
+      <c r="G63" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="H63" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="I63" s="191"/>
-      <c r="J63" s="192"/>
-      <c r="K63" s="192"/>
+      <c r="I63" s="127"/>
+      <c r="J63" s="128"/>
+      <c r="K63" s="128"/>
     </row>
     <row r="64" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
       <c r="B64" s="23"/>
       <c r="C64" s="24"/>
       <c r="D64" s="25"/>
-      <c r="E64" s="189"/>
-      <c r="F64" s="190"/>
-      <c r="G64" s="190" t="s">
-        <v>2</v>
-      </c>
-      <c r="H64" s="190"/>
-      <c r="I64" s="191"/>
-      <c r="J64" s="192"/>
-      <c r="K64" s="192"/>
+      <c r="E64" s="125"/>
+      <c r="F64" s="126"/>
+      <c r="G64" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="H64" s="126"/>
+      <c r="I64" s="127"/>
+      <c r="J64" s="128"/>
+      <c r="K64" s="128"/>
     </row>
     <row r="65" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
@@ -4968,30 +4921,30 @@
       <c r="D65" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E65" s="189">
-        <v>2</v>
-      </c>
-      <c r="F65" s="190"/>
-      <c r="G65" s="190"/>
-      <c r="H65" s="190"/>
-      <c r="I65" s="191" t="s">
+      <c r="E65" s="125">
+        <v>2</v>
+      </c>
+      <c r="F65" s="126"/>
+      <c r="G65" s="126"/>
+      <c r="H65" s="126"/>
+      <c r="I65" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="J65" s="192"/>
-      <c r="K65" s="192"/>
+      <c r="J65" s="128"/>
+      <c r="K65" s="128"/>
     </row>
     <row r="66" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="23"/>
       <c r="B66" s="23"/>
       <c r="C66" s="24"/>
       <c r="D66" s="25"/>
-      <c r="E66" s="189"/>
-      <c r="F66" s="190"/>
-      <c r="G66" s="190"/>
-      <c r="H66" s="190"/>
-      <c r="I66" s="191"/>
-      <c r="J66" s="192"/>
-      <c r="K66" s="192"/>
+      <c r="E66" s="125"/>
+      <c r="F66" s="126"/>
+      <c r="G66" s="126"/>
+      <c r="H66" s="126"/>
+      <c r="I66" s="127"/>
+      <c r="J66" s="128"/>
+      <c r="K66" s="128"/>
     </row>
     <row r="67" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
@@ -5004,30 +4957,30 @@
       <c r="D67" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E67" s="193">
+      <c r="E67" s="129">
         <v>3</v>
       </c>
-      <c r="F67" s="194"/>
-      <c r="G67" s="194"/>
-      <c r="H67" s="195" t="s">
+      <c r="F67" s="195"/>
+      <c r="G67" s="195"/>
+      <c r="H67" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="I67" s="195"/>
-      <c r="J67" s="192"/>
-      <c r="K67" s="192"/>
+      <c r="I67" s="130"/>
+      <c r="J67" s="128"/>
+      <c r="K67" s="128"/>
     </row>
     <row r="68" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="27"/>
       <c r="B68" s="27"/>
       <c r="C68" s="26"/>
       <c r="D68" s="26"/>
-      <c r="E68" s="193"/>
-      <c r="F68" s="195"/>
-      <c r="G68" s="195"/>
-      <c r="H68" s="195"/>
-      <c r="I68" s="195"/>
-      <c r="J68" s="192"/>
-      <c r="K68" s="192"/>
+      <c r="E68" s="129"/>
+      <c r="F68" s="130"/>
+      <c r="G68" s="130"/>
+      <c r="H68" s="130"/>
+      <c r="I68" s="130"/>
+      <c r="J68" s="128"/>
+      <c r="K68" s="128"/>
     </row>
     <row r="69" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
@@ -5040,34 +4993,34 @@
       <c r="D69" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="193">
+      <c r="E69" s="129">
         <v>4</v>
       </c>
-      <c r="F69" s="195"/>
-      <c r="G69" s="195"/>
-      <c r="H69" s="195"/>
-      <c r="I69" s="195" t="s">
+      <c r="F69" s="130"/>
+      <c r="G69" s="130"/>
+      <c r="H69" s="130"/>
+      <c r="I69" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="J69" s="192"/>
-      <c r="K69" s="192"/>
+      <c r="J69" s="128"/>
+      <c r="K69" s="128"/>
     </row>
     <row r="70" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="27"/>
       <c r="B70" s="27"/>
       <c r="C70" s="26"/>
       <c r="D70" s="26"/>
-      <c r="E70" s="193"/>
-      <c r="F70" s="195"/>
-      <c r="G70" s="195"/>
-      <c r="H70" s="195" t="s">
-        <v>2</v>
-      </c>
-      <c r="I70" s="195" t="s">
-        <v>2</v>
-      </c>
-      <c r="J70" s="192"/>
-      <c r="K70" s="192"/>
+      <c r="E70" s="129"/>
+      <c r="F70" s="130"/>
+      <c r="G70" s="130"/>
+      <c r="H70" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="I70" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="J70" s="128"/>
+      <c r="K70" s="128"/>
     </row>
     <row r="71" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
@@ -5080,17 +5033,17 @@
       <c r="D71" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E71" s="193">
+      <c r="E71" s="129">
         <v>5</v>
       </c>
-      <c r="F71" s="194"/>
-      <c r="G71" s="194"/>
-      <c r="H71" s="195" t="s">
+      <c r="F71" s="195"/>
+      <c r="G71" s="195"/>
+      <c r="H71" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="I71" s="195"/>
-      <c r="J71" s="192"/>
-      <c r="K71" s="192"/>
+      <c r="I71" s="130"/>
+      <c r="J71" s="128"/>
+      <c r="K71" s="128"/>
     </row>
     <row r="72" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
@@ -5099,17 +5052,17 @@
       <c r="B72" s="27"/>
       <c r="C72" s="26"/>
       <c r="D72" s="26"/>
-      <c r="E72" s="196"/>
-      <c r="F72" s="195"/>
-      <c r="G72" s="195"/>
-      <c r="H72" s="195" t="s">
-        <v>2</v>
-      </c>
-      <c r="I72" s="195" t="s">
-        <v>2</v>
-      </c>
-      <c r="J72" s="192"/>
-      <c r="K72" s="192"/>
+      <c r="E72" s="131"/>
+      <c r="F72" s="130"/>
+      <c r="G72" s="130"/>
+      <c r="H72" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="I72" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="J72" s="128"/>
+      <c r="K72" s="128"/>
     </row>
     <row r="73" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
@@ -5122,17 +5075,17 @@
       <c r="D73" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E73" s="193">
+      <c r="E73" s="129">
         <v>6</v>
       </c>
-      <c r="F73" s="195"/>
-      <c r="G73" s="195"/>
-      <c r="H73" s="195"/>
-      <c r="I73" s="195" t="s">
+      <c r="F73" s="130"/>
+      <c r="G73" s="130"/>
+      <c r="H73" s="130"/>
+      <c r="I73" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="192"/>
-      <c r="K73" s="192"/>
+      <c r="J73" s="128"/>
+      <c r="K73" s="128"/>
     </row>
     <row r="74" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="27"/>
@@ -5141,19 +5094,19 @@
       <c r="D74" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E74" s="193" t="s">
-        <v>2</v>
-      </c>
-      <c r="F74" s="195"/>
-      <c r="G74" s="195"/>
-      <c r="H74" s="195" t="s">
-        <v>2</v>
-      </c>
-      <c r="I74" s="195" t="s">
-        <v>2</v>
-      </c>
-      <c r="J74" s="192"/>
-      <c r="K74" s="192"/>
+      <c r="E74" s="129" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="130"/>
+      <c r="G74" s="130"/>
+      <c r="H74" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="I74" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="J74" s="128"/>
+      <c r="K74" s="128"/>
     </row>
     <row r="75" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
@@ -5166,17 +5119,17 @@
       <c r="D75" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E75" s="193">
+      <c r="E75" s="129">
         <v>7</v>
       </c>
-      <c r="F75" s="194"/>
-      <c r="G75" s="194"/>
-      <c r="H75" s="195" t="s">
+      <c r="F75" s="195"/>
+      <c r="G75" s="195"/>
+      <c r="H75" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="I75" s="195"/>
-      <c r="J75" s="192"/>
-      <c r="K75" s="192"/>
+      <c r="I75" s="130"/>
+      <c r="J75" s="128"/>
+      <c r="K75" s="128"/>
     </row>
     <row r="76" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="27"/>
@@ -5185,13 +5138,13 @@
       <c r="D76" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E76" s="195"/>
-      <c r="F76" s="193"/>
-      <c r="G76" s="195"/>
-      <c r="H76" s="195"/>
-      <c r="I76" s="195"/>
-      <c r="J76" s="192"/>
-      <c r="K76" s="192"/>
+      <c r="E76" s="130"/>
+      <c r="F76" s="129"/>
+      <c r="G76" s="130"/>
+      <c r="H76" s="130"/>
+      <c r="I76" s="130"/>
+      <c r="J76" s="128"/>
+      <c r="K76" s="128"/>
     </row>
     <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="27"/>
@@ -5399,19 +5352,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="F71:G71"/>
@@ -5422,6 +5362,19 @@
     <mergeCell ref="E59:I59"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0" top="0.19685039370078741" bottom="0" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>